<commit_message>
Organized scripts; added early base for game ui
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="300">
   <si>
     <t>Date:</t>
   </si>
@@ -1498,6 +1498,21 @@
   </si>
   <si>
     <t>Looking into UI design for similar games (Realm of the Mad God)</t>
+  </si>
+  <si>
+    <t>UI Design</t>
+  </si>
+  <si>
+    <t>First pass of what UI will look like</t>
+  </si>
+  <si>
+    <t>Designing requirements for UI</t>
+  </si>
+  <si>
+    <t>Creation of Wizard images</t>
+  </si>
+  <si>
+    <t>Maknig the sprites for the wizard's animations</t>
   </si>
 </sst>
 </file>
@@ -2254,12 +2269,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
@@ -3255,9 +3270,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3301,7 +3316,7 @@
       <c r="C3" s="57"/>
       <c r="H3" s="79">
         <f>SUM(G12:G120)</f>
-        <v>-0.67569444444444438</v>
+        <v>-0.68611111111111101</v>
       </c>
       <c r="I3" t="s">
         <v>187</v>
@@ -3415,9 +3430,12 @@
       <c r="D12" s="5">
         <v>0.67569444444444438</v>
       </c>
+      <c r="E12" s="5">
+        <v>0.68472222222222223</v>
+      </c>
       <c r="G12" s="8">
         <f>(E12-D12)-(F12/1440)</f>
-        <v>-0.67569444444444438</v>
+        <v>9.0277777777778567E-3</v>
       </c>
       <c r="H12" t="s">
         <v>293</v>
@@ -3431,21 +3449,69 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
+      <c r="C13" s="3">
+        <v>42110</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="G13" s="8">
         <f t="shared" ref="G13:G76" si="0">(E13-D13)-(F13/1440)</f>
-        <v>0</v>
+        <v>2.2916666666666696E-2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>295</v>
+      </c>
+      <c r="I13" t="s">
+        <v>219</v>
+      </c>
+      <c r="J13" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="3">
+        <v>42114</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.65625</v>
+      </c>
       <c r="G14" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.375E-2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>167</v>
+      </c>
+      <c r="I14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <v>42118</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.81180555555555556</v>
+      </c>
       <c r="G15" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.81180555555555556</v>
+      </c>
+      <c r="H15" t="s">
+        <v>298</v>
+      </c>
+      <c r="J15" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -5996,7 +6062,7 @@
       <c r="P10" s="110"/>
     </row>
     <row r="11" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="114" t="s">
+      <c r="C11" s="111" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="110"/>
@@ -6051,7 +6117,7 @@
       <c r="O14" s="110"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="111" t="s">
+      <c r="C15" s="112" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="110"/>
@@ -6093,7 +6159,7 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="113" t="s">
+      <c r="C18" s="114" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="110"/>
@@ -6112,7 +6178,7 @@
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="112" t="s">
+      <c r="D19" s="113" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="110"/>
@@ -6129,7 +6195,7 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
-      <c r="C20" s="112" t="s">
+      <c r="C20" s="113" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="110"/>
@@ -6243,7 +6309,7 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
-      <c r="C26" s="112" t="s">
+      <c r="C26" s="113" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="110"/>
@@ -6304,7 +6370,7 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="111" t="s">
+      <c r="C32" s="112" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="110"/>
@@ -6336,7 +6402,7 @@
       <c r="N34" s="110"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C35" s="111" t="s">
+      <c r="C35" s="112" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="110"/>
@@ -6368,7 +6434,7 @@
       <c r="N37" s="110"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C38" s="111" t="s">
+      <c r="C38" s="112" t="s">
         <v>25</v>
       </c>
       <c r="D38" s="110"/>
@@ -6385,12 +6451,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D25:Q25"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="B7:P7"/>
-    <mergeCell ref="B10:P10"/>
-    <mergeCell ref="B12:P12"/>
     <mergeCell ref="C34:N34"/>
     <mergeCell ref="C35:N35"/>
     <mergeCell ref="C37:N37"/>
@@ -6407,6 +6467,12 @@
     <mergeCell ref="D22:N22"/>
     <mergeCell ref="D23:Q23"/>
     <mergeCell ref="D24:Q24"/>
+    <mergeCell ref="D25:Q25"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="B10:P10"/>
+    <mergeCell ref="B12:P12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementation of wizard class animations
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="306">
   <si>
     <t>Date:</t>
   </si>
@@ -1513,6 +1513,24 @@
   </si>
   <si>
     <t>Maknig the sprites for the wizard's animations</t>
+  </si>
+  <si>
+    <t>UI Base (Game mode)</t>
+  </si>
+  <si>
+    <t>Creation of base component design for displaying player information</t>
+  </si>
+  <si>
+    <t>Wizard Animations (Idle/Walknig)</t>
+  </si>
+  <si>
+    <t>Asset Creation</t>
+  </si>
+  <si>
+    <t>Creation of in-game assets</t>
+  </si>
+  <si>
+    <t>Making the idle and walking animations for the wizard class</t>
   </si>
 </sst>
 </file>
@@ -2269,12 +2287,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
@@ -3270,9 +3288,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3316,7 +3334,7 @@
       <c r="C3" s="57"/>
       <c r="H3" s="79">
         <f>SUM(G12:G120)</f>
-        <v>-0.68611111111111101</v>
+        <v>-7.3611111111111016E-2</v>
       </c>
       <c r="I3" t="s">
         <v>187</v>
@@ -3501,116 +3519,155 @@
         <v>42118</v>
       </c>
       <c r="D15" s="5">
-        <v>0.81180555555555556</v>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.99583333333333324</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="0"/>
-        <v>-0.81180555555555556</v>
+        <v>7.9166666666666607E-2</v>
       </c>
       <c r="H15" t="s">
         <v>298</v>
       </c>
+      <c r="I15" t="s">
+        <v>303</v>
+      </c>
       <c r="J15" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="3">
+        <v>42119</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.99652777777777779</v>
+      </c>
       <c r="G16" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+        <v>7.986111111111116E-2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>300</v>
+      </c>
+      <c r="I16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="3">
+        <v>42120</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.35833333333333334</v>
+      </c>
       <c r="G17" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+        <v>-0.35833333333333334</v>
+      </c>
+      <c r="H17" t="s">
+        <v>302</v>
+      </c>
+      <c r="I17" t="s">
+        <v>303</v>
+      </c>
+      <c r="J17" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G18" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G19" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G20" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G21" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G22" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G23" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G24" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G25" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G26" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G27" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G28" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G29" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G30" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G31" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G32" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5074,8 +5131,8 @@
   <dimension ref="A1:F119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A80" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5296,7 +5353,12 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="26"/>
+      <c r="C28" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="23" t="s">
@@ -6062,7 +6124,7 @@
       <c r="P10" s="110"/>
     </row>
     <row r="11" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="111" t="s">
+      <c r="C11" s="114" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="110"/>
@@ -6117,7 +6179,7 @@
       <c r="O14" s="110"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="112" t="s">
+      <c r="C15" s="111" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="110"/>
@@ -6159,7 +6221,7 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="114" t="s">
+      <c r="C18" s="113" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="110"/>
@@ -6178,7 +6240,7 @@
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="113" t="s">
+      <c r="D19" s="112" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="110"/>
@@ -6195,7 +6257,7 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
-      <c r="C20" s="113" t="s">
+      <c r="C20" s="112" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="110"/>
@@ -6309,7 +6371,7 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
-      <c r="C26" s="113" t="s">
+      <c r="C26" s="112" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="110"/>
@@ -6370,7 +6432,7 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="112" t="s">
+      <c r="C32" s="111" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="110"/>
@@ -6402,7 +6464,7 @@
       <c r="N34" s="110"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C35" s="112" t="s">
+      <c r="C35" s="111" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="110"/>
@@ -6434,7 +6496,7 @@
       <c r="N37" s="110"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C38" s="112" t="s">
+      <c r="C38" s="111" t="s">
         <v>25</v>
       </c>
       <c r="D38" s="110"/>
@@ -6451,6 +6513,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="D25:Q25"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="B10:P10"/>
+    <mergeCell ref="B12:P12"/>
     <mergeCell ref="C34:N34"/>
     <mergeCell ref="C35:N35"/>
     <mergeCell ref="C37:N37"/>
@@ -6467,12 +6535,6 @@
     <mergeCell ref="D22:N22"/>
     <mergeCell ref="D23:Q23"/>
     <mergeCell ref="D24:Q24"/>
-    <mergeCell ref="D25:Q25"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="B7:P7"/>
-    <mergeCell ref="B10:P10"/>
-    <mergeCell ref="B12:P12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1"/>

</xml_diff>

<commit_message>
Added charge enemy images (idle and moving); added title screen UI prefab to splash scene;
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="308">
   <si>
     <t>Date:</t>
   </si>
@@ -1530,7 +1530,14 @@
     <t>Creation of in-game assets</t>
   </si>
   <si>
-    <t>Making the idle and walking animations for the wizard class</t>
+    <t>Making the idle and walking animations for the wizard class;
+bring animations into Unity</t>
+  </si>
+  <si>
+    <t>Menu Implementation</t>
+  </si>
+  <si>
+    <t>Creation of scenes that comprise in-game menus (title, character select)</t>
   </si>
 </sst>
 </file>
@@ -2019,7 +2026,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2285,6 +2292,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -3286,11 +3296,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3333,8 +3343,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="57"/>
       <c r="H3" s="79">
-        <f>SUM(G12:G120)</f>
-        <v>0.34305555555555567</v>
+        <f>SUM(G12:G119)</f>
+        <v>-0.44861111111111096</v>
       </c>
       <c r="I3" t="s">
         <v>187</v>
@@ -3345,9 +3355,9 @@
         <v>184</v>
       </c>
       <c r="C4" s="27"/>
-      <c r="H4" s="80">
+      <c r="H4" s="80" t="e">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>8.2333333333333325</v>
+        <v>#NUM!</v>
       </c>
       <c r="I4" t="s">
         <v>187</v>
@@ -3477,7 +3487,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" ref="G13:G76" si="0">(E13-D13)-(F13/1440)</f>
+        <f t="shared" ref="G13:G75" si="0">(E13-D13)-(F13/1440)</f>
         <v>2.2916666666666696E-2</v>
       </c>
       <c r="H13" t="s">
@@ -3562,7 +3572,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C17" s="3">
         <v>42120</v>
       </c>
@@ -3582,14 +3592,29 @@
       <c r="I17" t="s">
         <v>303</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="110" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="3">
+        <v>42122</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="G18" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.79166666666666663</v>
+      </c>
+      <c r="H18" t="s">
+        <v>306</v>
+      </c>
+      <c r="I18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
@@ -3936,13 +3961,13 @@
     </row>
     <row r="76" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G76" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G76:G119" si="1">(E76-D76)-(F76/1440)</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G77" s="8">
-        <f t="shared" ref="G77:G120" si="1">(E77-D77)-(F77/1440)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4194,12 +4219,6 @@
     </row>
     <row r="119" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G119" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G120" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4217,7 +4236,7 @@
           <x14:formula1>
             <xm:f>Menu!$C$11:$C$28</xm:f>
           </x14:formula1>
-          <xm:sqref>I12:I120</xm:sqref>
+          <xm:sqref>I12:I119</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6062,42 +6081,42 @@
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="110"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="111"/>
+      <c r="M6" s="111"/>
+      <c r="N6" s="111"/>
+      <c r="O6" s="111"/>
+      <c r="P6" s="111"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="110"/>
-      <c r="N7" s="110"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="110"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="111"/>
+      <c r="M7" s="111"/>
+      <c r="N7" s="111"/>
+      <c r="O7" s="111"/>
+      <c r="P7" s="111"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -6108,55 +6127,55 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="110" t="s">
+      <c r="B10" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="110"/>
-      <c r="D10" s="110"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="110"/>
-      <c r="K10" s="110"/>
-      <c r="L10" s="110"/>
-      <c r="M10" s="110"/>
-      <c r="N10" s="110"/>
-      <c r="O10" s="110"/>
-      <c r="P10" s="110"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="111"/>
+      <c r="K10" s="111"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="111"/>
+      <c r="N10" s="111"/>
+      <c r="O10" s="111"/>
+      <c r="P10" s="111"/>
     </row>
     <row r="11" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="114" t="s">
+      <c r="C11" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="110"/>
-      <c r="K11" s="110"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="111"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="110" t="s">
+      <c r="B12" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="110"/>
-      <c r="D12" s="110"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="110"/>
-      <c r="H12" s="110"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="110"/>
-      <c r="K12" s="110"/>
-      <c r="L12" s="110"/>
-      <c r="M12" s="110"/>
-      <c r="N12" s="110"/>
-      <c r="O12" s="110"/>
-      <c r="P12" s="110"/>
+      <c r="C12" s="111"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="111"/>
+      <c r="M12" s="111"/>
+      <c r="N12" s="111"/>
+      <c r="O12" s="111"/>
+      <c r="P12" s="111"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="11" t="s">
@@ -6164,36 +6183,36 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="110"/>
-      <c r="L14" s="110"/>
-      <c r="M14" s="110"/>
-      <c r="N14" s="110"/>
-      <c r="O14" s="110"/>
+      <c r="C14" s="111"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="111"/>
+      <c r="K14" s="111"/>
+      <c r="L14" s="111"/>
+      <c r="M14" s="111"/>
+      <c r="N14" s="111"/>
+      <c r="O14" s="111"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="111" t="s">
+      <c r="C15" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="110"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="110"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="111"/>
+      <c r="H15" s="111"/>
+      <c r="I15" s="111"/>
+      <c r="J15" s="111"/>
+      <c r="K15" s="111"/>
+      <c r="L15" s="111"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16" s="12"/>
@@ -6224,187 +6243,187 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="113" t="s">
+      <c r="C18" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="110"/>
-      <c r="E18" s="110"/>
-      <c r="F18" s="110"/>
-      <c r="G18" s="110"/>
-      <c r="H18" s="110"/>
-      <c r="I18" s="110"/>
-      <c r="J18" s="110"/>
-      <c r="K18" s="110"/>
-      <c r="L18" s="110"/>
-      <c r="M18" s="110"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="111"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="111"/>
+      <c r="I18" s="111"/>
+      <c r="J18" s="111"/>
+      <c r="K18" s="111"/>
+      <c r="L18" s="111"/>
+      <c r="M18" s="111"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="112" t="s">
+      <c r="D19" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="110"/>
-      <c r="J19" s="110"/>
-      <c r="K19" s="110"/>
-      <c r="L19" s="110"/>
-      <c r="M19" s="110"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="111"/>
+      <c r="K19" s="111"/>
+      <c r="L19" s="111"/>
+      <c r="M19" s="111"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
-      <c r="C20" s="112" t="s">
+      <c r="C20" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="110"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="110"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="110"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="110"/>
-      <c r="L20" s="110"/>
-      <c r="M20" s="110"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="111"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="111"/>
+      <c r="I20" s="111"/>
+      <c r="J20" s="111"/>
+      <c r="K20" s="111"/>
+      <c r="L20" s="111"/>
+      <c r="M20" s="111"/>
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="110" t="s">
+      <c r="D21" s="111" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110"/>
-      <c r="G21" s="110"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="110"/>
-      <c r="K21" s="110"/>
-      <c r="L21" s="110"/>
-      <c r="M21" s="110"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="111"/>
+      <c r="M21" s="111"/>
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="110" t="s">
+      <c r="D22" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110"/>
-      <c r="J22" s="110"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="110"/>
-      <c r="M22" s="110"/>
-      <c r="N22" s="110"/>
+      <c r="E22" s="111"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="111"/>
+      <c r="H22" s="111"/>
+      <c r="I22" s="111"/>
+      <c r="J22" s="111"/>
+      <c r="K22" s="111"/>
+      <c r="L22" s="111"/>
+      <c r="M22" s="111"/>
+      <c r="N22" s="111"/>
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="110" t="s">
+      <c r="D23" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="110"/>
-      <c r="F23" s="110"/>
-      <c r="G23" s="110"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="110"/>
-      <c r="K23" s="110"/>
-      <c r="L23" s="110"/>
-      <c r="M23" s="110"/>
-      <c r="N23" s="110"/>
-      <c r="O23" s="110"/>
-      <c r="P23" s="110"/>
-      <c r="Q23" s="110"/>
+      <c r="E23" s="111"/>
+      <c r="F23" s="111"/>
+      <c r="G23" s="111"/>
+      <c r="H23" s="111"/>
+      <c r="I23" s="111"/>
+      <c r="J23" s="111"/>
+      <c r="K23" s="111"/>
+      <c r="L23" s="111"/>
+      <c r="M23" s="111"/>
+      <c r="N23" s="111"/>
+      <c r="O23" s="111"/>
+      <c r="P23" s="111"/>
+      <c r="Q23" s="111"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="110" t="s">
+      <c r="D24" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="110"/>
-      <c r="F24" s="110"/>
-      <c r="G24" s="110"/>
-      <c r="H24" s="110"/>
-      <c r="I24" s="110"/>
-      <c r="J24" s="110"/>
-      <c r="K24" s="110"/>
-      <c r="L24" s="110"/>
-      <c r="M24" s="110"/>
-      <c r="N24" s="110"/>
-      <c r="O24" s="110"/>
-      <c r="P24" s="110"/>
-      <c r="Q24" s="110"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="111"/>
+      <c r="H24" s="111"/>
+      <c r="I24" s="111"/>
+      <c r="J24" s="111"/>
+      <c r="K24" s="111"/>
+      <c r="L24" s="111"/>
+      <c r="M24" s="111"/>
+      <c r="N24" s="111"/>
+      <c r="O24" s="111"/>
+      <c r="P24" s="111"/>
+      <c r="Q24" s="111"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="110" t="s">
+      <c r="D25" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="110"/>
-      <c r="F25" s="110"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="110"/>
-      <c r="K25" s="110"/>
-      <c r="L25" s="110"/>
-      <c r="M25" s="110"/>
-      <c r="N25" s="110"/>
-      <c r="O25" s="110"/>
-      <c r="P25" s="110"/>
-      <c r="Q25" s="110"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="111"/>
+      <c r="G25" s="111"/>
+      <c r="H25" s="111"/>
+      <c r="I25" s="111"/>
+      <c r="J25" s="111"/>
+      <c r="K25" s="111"/>
+      <c r="L25" s="111"/>
+      <c r="M25" s="111"/>
+      <c r="N25" s="111"/>
+      <c r="O25" s="111"/>
+      <c r="P25" s="111"/>
+      <c r="Q25" s="111"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
-      <c r="C26" s="112" t="s">
+      <c r="C26" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="110"/>
-      <c r="E26" s="110"/>
-      <c r="F26" s="110"/>
-      <c r="G26" s="110"/>
-      <c r="H26" s="110"/>
-      <c r="I26" s="110"/>
-      <c r="J26" s="110"/>
-      <c r="K26" s="110"/>
-      <c r="L26" s="110"/>
-      <c r="M26" s="110"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
+      <c r="G26" s="111"/>
+      <c r="H26" s="111"/>
+      <c r="I26" s="111"/>
+      <c r="J26" s="111"/>
+      <c r="K26" s="111"/>
+      <c r="L26" s="111"/>
+      <c r="M26" s="111"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="110" t="s">
+      <c r="D27" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="110"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="110"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="110"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="110"/>
-      <c r="L27" s="110"/>
-      <c r="M27" s="110"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="111"/>
+      <c r="H27" s="111"/>
+      <c r="I27" s="111"/>
+      <c r="J27" s="111"/>
+      <c r="K27" s="111"/>
+      <c r="L27" s="111"/>
+      <c r="M27" s="111"/>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
     </row>
@@ -6435,84 +6454,84 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="111" t="s">
+      <c r="C32" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="110"/>
-      <c r="E32" s="110"/>
-      <c r="F32" s="110"/>
-      <c r="G32" s="110"/>
-      <c r="H32" s="110"/>
-      <c r="I32" s="110"/>
-      <c r="J32" s="110"/>
-      <c r="K32" s="110"/>
-      <c r="L32" s="110"/>
-      <c r="M32" s="110"/>
-      <c r="N32" s="110"/>
+      <c r="D32" s="111"/>
+      <c r="E32" s="111"/>
+      <c r="F32" s="111"/>
+      <c r="G32" s="111"/>
+      <c r="H32" s="111"/>
+      <c r="I32" s="111"/>
+      <c r="J32" s="111"/>
+      <c r="K32" s="111"/>
+      <c r="L32" s="111"/>
+      <c r="M32" s="111"/>
+      <c r="N32" s="111"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C34" s="110" t="s">
+      <c r="C34" s="111" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="110"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="110"/>
-      <c r="I34" s="110"/>
-      <c r="J34" s="110"/>
-      <c r="K34" s="110"/>
-      <c r="L34" s="110"/>
-      <c r="M34" s="110"/>
-      <c r="N34" s="110"/>
+      <c r="D34" s="111"/>
+      <c r="E34" s="111"/>
+      <c r="F34" s="111"/>
+      <c r="G34" s="111"/>
+      <c r="H34" s="111"/>
+      <c r="I34" s="111"/>
+      <c r="J34" s="111"/>
+      <c r="K34" s="111"/>
+      <c r="L34" s="111"/>
+      <c r="M34" s="111"/>
+      <c r="N34" s="111"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C35" s="111" t="s">
+      <c r="C35" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="110"/>
-      <c r="E35" s="110"/>
-      <c r="F35" s="110"/>
-      <c r="G35" s="110"/>
-      <c r="H35" s="110"/>
-      <c r="I35" s="110"/>
-      <c r="J35" s="110"/>
-      <c r="K35" s="110"/>
-      <c r="L35" s="110"/>
-      <c r="M35" s="110"/>
-      <c r="N35" s="110"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="111"/>
+      <c r="G35" s="111"/>
+      <c r="H35" s="111"/>
+      <c r="I35" s="111"/>
+      <c r="J35" s="111"/>
+      <c r="K35" s="111"/>
+      <c r="L35" s="111"/>
+      <c r="M35" s="111"/>
+      <c r="N35" s="111"/>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C37" s="110" t="s">
+      <c r="C37" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="110"/>
-      <c r="E37" s="110"/>
-      <c r="F37" s="110"/>
-      <c r="G37" s="110"/>
-      <c r="H37" s="110"/>
-      <c r="I37" s="110"/>
-      <c r="J37" s="110"/>
-      <c r="K37" s="110"/>
-      <c r="L37" s="110"/>
-      <c r="M37" s="110"/>
-      <c r="N37" s="110"/>
+      <c r="D37" s="111"/>
+      <c r="E37" s="111"/>
+      <c r="F37" s="111"/>
+      <c r="G37" s="111"/>
+      <c r="H37" s="111"/>
+      <c r="I37" s="111"/>
+      <c r="J37" s="111"/>
+      <c r="K37" s="111"/>
+      <c r="L37" s="111"/>
+      <c r="M37" s="111"/>
+      <c r="N37" s="111"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C38" s="111" t="s">
+      <c r="C38" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="110"/>
-      <c r="E38" s="110"/>
-      <c r="F38" s="110"/>
-      <c r="G38" s="110"/>
-      <c r="H38" s="110"/>
-      <c r="I38" s="110"/>
-      <c r="J38" s="110"/>
-      <c r="K38" s="110"/>
-      <c r="L38" s="110"/>
-      <c r="M38" s="110"/>
-      <c r="N38" s="110"/>
+      <c r="D38" s="111"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="111"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="111"/>
+      <c r="I38" s="111"/>
+      <c r="J38" s="111"/>
+      <c r="K38" s="111"/>
+      <c r="L38" s="111"/>
+      <c r="M38" s="111"/>
+      <c r="N38" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="22">

</xml_diff>

<commit_message>
Player controller script now reads stats from char save file; game mode UI updated to read experience
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="311">
   <si>
     <t>Date:</t>
   </si>
@@ -1538,6 +1538,15 @@
   </si>
   <si>
     <t>Creation of scenes that comprise in-game menus (title, character select)</t>
+  </si>
+  <si>
+    <t>Charge Enemy Animations (Idle/Moving)</t>
+  </si>
+  <si>
+    <t>UI Fixing</t>
+  </si>
+  <si>
+    <t>Changing Game Mode UI implementation to match the updated method of storing character stats</t>
   </si>
 </sst>
 </file>
@@ -3298,9 +3307,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3344,7 +3353,7 @@
       <c r="C3" s="57"/>
       <c r="H3" s="79">
         <f>SUM(G12:G119)</f>
-        <v>-0.44861111111111096</v>
+        <v>0.46180555555555575</v>
       </c>
       <c r="I3" t="s">
         <v>187</v>
@@ -3355,9 +3364,9 @@
         <v>184</v>
       </c>
       <c r="C4" s="27"/>
-      <c r="H4" s="80" t="e">
+      <c r="H4" s="80">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>#NUM!</v>
+        <v>11.083333333333334</v>
       </c>
       <c r="I4" t="s">
         <v>187</v>
@@ -3603,9 +3612,12 @@
       <c r="D18" s="5">
         <v>0.79166666666666663</v>
       </c>
+      <c r="E18" s="5">
+        <v>0.8125</v>
+      </c>
       <c r="G18" s="8">
         <f t="shared" si="0"/>
-        <v>-0.79166666666666663</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="H18" t="s">
         <v>306</v>
@@ -3618,15 +3630,48 @@
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="3">
+        <v>42122</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.8125</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="G19" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>308</v>
+      </c>
+      <c r="I19" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="3">
+        <v>42123</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.3125</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.38958333333333334</v>
+      </c>
       <c r="G20" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.7083333333333337E-2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>309</v>
+      </c>
+      <c r="I20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added animations for berserk enemy type; actually committed shortcut script this time :P; updated berserk enemy scripts to avoid animation component access error
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Project Info" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="318">
   <si>
     <t>Date:</t>
   </si>
@@ -1547,6 +1547,28 @@
   </si>
   <si>
     <t>Changing Game Mode UI implementation to match the updated method of storing character stats</t>
+  </si>
+  <si>
+    <t>Berserk Enemy Animations (Idle/Moving)</t>
+  </si>
+  <si>
+    <t>Creating Charge Enemy sprites</t>
+  </si>
+  <si>
+    <t>Creating Berserk Enemy sprites</t>
+  </si>
+  <si>
+    <t>Charge Enemy Animations</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>For some enemy types that used the charge enemy script but didn't have the charge enemy animation components, nullreference errors where thrown for each enemy present in the scene trying to access nonexistent animation components
+RESOLVED: added a check for charge enemy script (and future enmy types with animations) to to see if animation components are needed or not</t>
   </si>
 </sst>
 </file>
@@ -2035,7 +2057,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2305,13 +2327,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
@@ -3305,11 +3330,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J119"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="11" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3352,8 +3377,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="57"/>
       <c r="H3" s="79">
-        <f>SUM(G12:G119)</f>
-        <v>0.46180555555555575</v>
+        <f>SUM(G12:G118)</f>
+        <v>0.47222222222222249</v>
       </c>
       <c r="I3" t="s">
         <v>187</v>
@@ -3366,7 +3391,7 @@
       <c r="C4" s="27"/>
       <c r="H4" s="80">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>11.083333333333334</v>
+        <v>11.333333333333334</v>
       </c>
       <c r="I4" t="s">
         <v>187</v>
@@ -3496,7 +3521,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" ref="G13:G75" si="0">(E13-D13)-(F13/1440)</f>
+        <f t="shared" ref="G13:G74" si="0">(E13-D13)-(F13/1440)</f>
         <v>2.2916666666666696E-2</v>
       </c>
       <c r="H13" t="s">
@@ -3649,6 +3674,9 @@
       <c r="I19" t="s">
         <v>303</v>
       </c>
+      <c r="J19" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="3">
@@ -3675,9 +3703,27 @@
       </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="3">
+        <v>42123</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="H21" t="s">
+        <v>311</v>
+      </c>
+      <c r="I21" t="s">
+        <v>303</v>
+      </c>
+      <c r="J21" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
@@ -4000,13 +4046,13 @@
     </row>
     <row r="75" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G75" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G75:G118" si="1">(E75-D75)-(F75/1440)</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G76" s="8">
-        <f t="shared" ref="G76:G119" si="1">(E76-D76)-(F76/1440)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4258,12 +4304,6 @@
     </row>
     <row r="118" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G118" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G119" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4281,7 +4321,7 @@
           <x14:formula1>
             <xm:f>Menu!$C$11:$C$28</xm:f>
           </x14:formula1>
-          <xm:sqref>I12:I119</xm:sqref>
+          <xm:sqref>I12:I118</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4293,9 +4333,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4340,7 +4380,7 @@
       <c r="C3" s="2"/>
       <c r="H3" s="79">
         <f>SUM(G12:G120)</f>
-        <v>0</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="I3" t="s">
         <v>187</v>
@@ -4355,7 +4395,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="80">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>0</v>
+        <v>16.416666666666668</v>
       </c>
       <c r="I4" t="s">
         <v>187</v>
@@ -4462,10 +4502,43 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="150.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>42123</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.68402777777777779</v>
+      </c>
       <c r="G12" s="8">
         <f>(E12-D12)-(F12/1440)</f>
-        <v>0</v>
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="H12" t="s">
+        <v>314</v>
+      </c>
+      <c r="I12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" t="s">
+        <v>264</v>
+      </c>
+      <c r="K12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" t="s">
+        <v>315</v>
+      </c>
+      <c r="N12" t="s">
+        <v>316</v>
+      </c>
+      <c r="O12" s="111" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -6126,42 +6199,42 @@
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
-      <c r="G6" s="111"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="111"/>
-      <c r="M6" s="111"/>
-      <c r="N6" s="111"/>
-      <c r="O6" s="111"/>
-      <c r="P6" s="111"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="112"/>
+      <c r="J6" s="112"/>
+      <c r="K6" s="112"/>
+      <c r="L6" s="112"/>
+      <c r="M6" s="112"/>
+      <c r="N6" s="112"/>
+      <c r="O6" s="112"/>
+      <c r="P6" s="112"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
-      <c r="L7" s="111"/>
-      <c r="M7" s="111"/>
-      <c r="N7" s="111"/>
-      <c r="O7" s="111"/>
-      <c r="P7" s="111"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="112"/>
+      <c r="J7" s="112"/>
+      <c r="K7" s="112"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="112"/>
+      <c r="O7" s="112"/>
+      <c r="P7" s="112"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -6172,55 +6245,55 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="111"/>
-      <c r="G10" s="111"/>
-      <c r="H10" s="111"/>
-      <c r="I10" s="111"/>
-      <c r="J10" s="111"/>
-      <c r="K10" s="111"/>
-      <c r="L10" s="111"/>
-      <c r="M10" s="111"/>
-      <c r="N10" s="111"/>
-      <c r="O10" s="111"/>
-      <c r="P10" s="111"/>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
+      <c r="G10" s="112"/>
+      <c r="H10" s="112"/>
+      <c r="I10" s="112"/>
+      <c r="J10" s="112"/>
+      <c r="K10" s="112"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="112"/>
+      <c r="O10" s="112"/>
+      <c r="P10" s="112"/>
     </row>
     <row r="11" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="115" t="s">
+      <c r="C11" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="111"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="111"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="112"/>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
+      <c r="K11" s="112"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="111" t="s">
+      <c r="B12" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="111"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="111"/>
-      <c r="L12" s="111"/>
-      <c r="M12" s="111"/>
-      <c r="N12" s="111"/>
-      <c r="O12" s="111"/>
-      <c r="P12" s="111"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="112"/>
+      <c r="K12" s="112"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="112"/>
+      <c r="O12" s="112"/>
+      <c r="P12" s="112"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="11" t="s">
@@ -6228,36 +6301,36 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="111" t="s">
+      <c r="B14" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="111"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="111"/>
-      <c r="H14" s="111"/>
-      <c r="I14" s="111"/>
-      <c r="J14" s="111"/>
-      <c r="K14" s="111"/>
-      <c r="L14" s="111"/>
-      <c r="M14" s="111"/>
-      <c r="N14" s="111"/>
-      <c r="O14" s="111"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="112"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="112"/>
+      <c r="K14" s="112"/>
+      <c r="L14" s="112"/>
+      <c r="M14" s="112"/>
+      <c r="N14" s="112"/>
+      <c r="O14" s="112"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="112" t="s">
+      <c r="C15" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="111"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="111"/>
-      <c r="H15" s="111"/>
-      <c r="I15" s="111"/>
-      <c r="J15" s="111"/>
-      <c r="K15" s="111"/>
-      <c r="L15" s="111"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="112"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16" s="12"/>
@@ -6288,187 +6361,187 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="114" t="s">
+      <c r="C18" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="111"/>
-      <c r="J18" s="111"/>
-      <c r="K18" s="111"/>
-      <c r="L18" s="111"/>
-      <c r="M18" s="111"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="112"/>
+      <c r="K18" s="112"/>
+      <c r="L18" s="112"/>
+      <c r="M18" s="112"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="113" t="s">
+      <c r="D19" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="111"/>
-      <c r="J19" s="111"/>
-      <c r="K19" s="111"/>
-      <c r="L19" s="111"/>
-      <c r="M19" s="111"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
+      <c r="K19" s="112"/>
+      <c r="L19" s="112"/>
+      <c r="M19" s="112"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
-      <c r="C20" s="113" t="s">
+      <c r="C20" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="111"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="111"/>
-      <c r="I20" s="111"/>
-      <c r="J20" s="111"/>
-      <c r="K20" s="111"/>
-      <c r="L20" s="111"/>
-      <c r="M20" s="111"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="112"/>
+      <c r="F20" s="112"/>
+      <c r="G20" s="112"/>
+      <c r="H20" s="112"/>
+      <c r="I20" s="112"/>
+      <c r="J20" s="112"/>
+      <c r="K20" s="112"/>
+      <c r="L20" s="112"/>
+      <c r="M20" s="112"/>
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="111" t="s">
+      <c r="D21" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="111"/>
-      <c r="F21" s="111"/>
-      <c r="G21" s="111"/>
-      <c r="H21" s="111"/>
-      <c r="I21" s="111"/>
-      <c r="J21" s="111"/>
-      <c r="K21" s="111"/>
-      <c r="L21" s="111"/>
-      <c r="M21" s="111"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="112"/>
+      <c r="M21" s="112"/>
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="111" t="s">
+      <c r="D22" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="111"/>
-      <c r="F22" s="111"/>
-      <c r="G22" s="111"/>
-      <c r="H22" s="111"/>
-      <c r="I22" s="111"/>
-      <c r="J22" s="111"/>
-      <c r="K22" s="111"/>
-      <c r="L22" s="111"/>
-      <c r="M22" s="111"/>
-      <c r="N22" s="111"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="112"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="112"/>
+      <c r="I22" s="112"/>
+      <c r="J22" s="112"/>
+      <c r="K22" s="112"/>
+      <c r="L22" s="112"/>
+      <c r="M22" s="112"/>
+      <c r="N22" s="112"/>
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="111" t="s">
+      <c r="D23" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="111"/>
-      <c r="H23" s="111"/>
-      <c r="I23" s="111"/>
-      <c r="J23" s="111"/>
-      <c r="K23" s="111"/>
-      <c r="L23" s="111"/>
-      <c r="M23" s="111"/>
-      <c r="N23" s="111"/>
-      <c r="O23" s="111"/>
-      <c r="P23" s="111"/>
-      <c r="Q23" s="111"/>
+      <c r="E23" s="112"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="112"/>
+      <c r="I23" s="112"/>
+      <c r="J23" s="112"/>
+      <c r="K23" s="112"/>
+      <c r="L23" s="112"/>
+      <c r="M23" s="112"/>
+      <c r="N23" s="112"/>
+      <c r="O23" s="112"/>
+      <c r="P23" s="112"/>
+      <c r="Q23" s="112"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="111" t="s">
+      <c r="D24" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111"/>
-      <c r="J24" s="111"/>
-      <c r="K24" s="111"/>
-      <c r="L24" s="111"/>
-      <c r="M24" s="111"/>
-      <c r="N24" s="111"/>
-      <c r="O24" s="111"/>
-      <c r="P24" s="111"/>
-      <c r="Q24" s="111"/>
+      <c r="E24" s="112"/>
+      <c r="F24" s="112"/>
+      <c r="G24" s="112"/>
+      <c r="H24" s="112"/>
+      <c r="I24" s="112"/>
+      <c r="J24" s="112"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="112"/>
+      <c r="M24" s="112"/>
+      <c r="N24" s="112"/>
+      <c r="O24" s="112"/>
+      <c r="P24" s="112"/>
+      <c r="Q24" s="112"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="111" t="s">
+      <c r="D25" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="111"/>
-      <c r="H25" s="111"/>
-      <c r="I25" s="111"/>
-      <c r="J25" s="111"/>
-      <c r="K25" s="111"/>
-      <c r="L25" s="111"/>
-      <c r="M25" s="111"/>
-      <c r="N25" s="111"/>
-      <c r="O25" s="111"/>
-      <c r="P25" s="111"/>
-      <c r="Q25" s="111"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="112"/>
+      <c r="G25" s="112"/>
+      <c r="H25" s="112"/>
+      <c r="I25" s="112"/>
+      <c r="J25" s="112"/>
+      <c r="K25" s="112"/>
+      <c r="L25" s="112"/>
+      <c r="M25" s="112"/>
+      <c r="N25" s="112"/>
+      <c r="O25" s="112"/>
+      <c r="P25" s="112"/>
+      <c r="Q25" s="112"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
-      <c r="C26" s="113" t="s">
+      <c r="C26" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="111"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
-      <c r="G26" s="111"/>
-      <c r="H26" s="111"/>
-      <c r="I26" s="111"/>
-      <c r="J26" s="111"/>
-      <c r="K26" s="111"/>
-      <c r="L26" s="111"/>
-      <c r="M26" s="111"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
+      <c r="G26" s="112"/>
+      <c r="H26" s="112"/>
+      <c r="I26" s="112"/>
+      <c r="J26" s="112"/>
+      <c r="K26" s="112"/>
+      <c r="L26" s="112"/>
+      <c r="M26" s="112"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="111" t="s">
+      <c r="D27" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="111"/>
-      <c r="H27" s="111"/>
-      <c r="I27" s="111"/>
-      <c r="J27" s="111"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="111"/>
-      <c r="M27" s="111"/>
+      <c r="E27" s="112"/>
+      <c r="F27" s="112"/>
+      <c r="G27" s="112"/>
+      <c r="H27" s="112"/>
+      <c r="I27" s="112"/>
+      <c r="J27" s="112"/>
+      <c r="K27" s="112"/>
+      <c r="L27" s="112"/>
+      <c r="M27" s="112"/>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
     </row>
@@ -6499,93 +6572,87 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="112" t="s">
+      <c r="C32" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="111"/>
-      <c r="E32" s="111"/>
-      <c r="F32" s="111"/>
-      <c r="G32" s="111"/>
-      <c r="H32" s="111"/>
-      <c r="I32" s="111"/>
-      <c r="J32" s="111"/>
-      <c r="K32" s="111"/>
-      <c r="L32" s="111"/>
-      <c r="M32" s="111"/>
-      <c r="N32" s="111"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="112"/>
+      <c r="F32" s="112"/>
+      <c r="G32" s="112"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="112"/>
+      <c r="J32" s="112"/>
+      <c r="K32" s="112"/>
+      <c r="L32" s="112"/>
+      <c r="M32" s="112"/>
+      <c r="N32" s="112"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C34" s="111" t="s">
+      <c r="C34" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="111"/>
-      <c r="E34" s="111"/>
-      <c r="F34" s="111"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="111"/>
-      <c r="I34" s="111"/>
-      <c r="J34" s="111"/>
-      <c r="K34" s="111"/>
-      <c r="L34" s="111"/>
-      <c r="M34" s="111"/>
-      <c r="N34" s="111"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="112"/>
+      <c r="H34" s="112"/>
+      <c r="I34" s="112"/>
+      <c r="J34" s="112"/>
+      <c r="K34" s="112"/>
+      <c r="L34" s="112"/>
+      <c r="M34" s="112"/>
+      <c r="N34" s="112"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C35" s="112" t="s">
+      <c r="C35" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="111"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="111"/>
-      <c r="I35" s="111"/>
-      <c r="J35" s="111"/>
-      <c r="K35" s="111"/>
-      <c r="L35" s="111"/>
-      <c r="M35" s="111"/>
-      <c r="N35" s="111"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="112"/>
+      <c r="G35" s="112"/>
+      <c r="H35" s="112"/>
+      <c r="I35" s="112"/>
+      <c r="J35" s="112"/>
+      <c r="K35" s="112"/>
+      <c r="L35" s="112"/>
+      <c r="M35" s="112"/>
+      <c r="N35" s="112"/>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C37" s="111" t="s">
+      <c r="C37" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="111"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="111"/>
-      <c r="G37" s="111"/>
-      <c r="H37" s="111"/>
-      <c r="I37" s="111"/>
-      <c r="J37" s="111"/>
-      <c r="K37" s="111"/>
-      <c r="L37" s="111"/>
-      <c r="M37" s="111"/>
-      <c r="N37" s="111"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="112"/>
+      <c r="F37" s="112"/>
+      <c r="G37" s="112"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="112"/>
+      <c r="J37" s="112"/>
+      <c r="K37" s="112"/>
+      <c r="L37" s="112"/>
+      <c r="M37" s="112"/>
+      <c r="N37" s="112"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C38" s="112" t="s">
+      <c r="C38" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="111"/>
-      <c r="E38" s="111"/>
-      <c r="F38" s="111"/>
-      <c r="G38" s="111"/>
-      <c r="H38" s="111"/>
-      <c r="I38" s="111"/>
-      <c r="J38" s="111"/>
-      <c r="K38" s="111"/>
-      <c r="L38" s="111"/>
-      <c r="M38" s="111"/>
-      <c r="N38" s="111"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="112"/>
+      <c r="F38" s="112"/>
+      <c r="G38" s="112"/>
+      <c r="H38" s="112"/>
+      <c r="I38" s="112"/>
+      <c r="J38" s="112"/>
+      <c r="K38" s="112"/>
+      <c r="L38" s="112"/>
+      <c r="M38" s="112"/>
+      <c r="N38" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D25:Q25"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="B7:P7"/>
-    <mergeCell ref="B10:P10"/>
-    <mergeCell ref="B12:P12"/>
     <mergeCell ref="C34:N34"/>
     <mergeCell ref="C35:N35"/>
     <mergeCell ref="C37:N37"/>
@@ -6602,6 +6669,12 @@
     <mergeCell ref="D22:N22"/>
     <mergeCell ref="D23:Q23"/>
     <mergeCell ref="D24:Q24"/>
+    <mergeCell ref="D25:Q25"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="B10:P10"/>
+    <mergeCell ref="B12:P12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1"/>

</xml_diff>

<commit_message>
...a bunch of stuff :P player saves write to file; quit button added to title screen/main menu; stat increases on level up (growth rates differ between classes); returned selected character stat display to main menu; game mode UI displays experience bar correctly now, HP values written on HP bar
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Info" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="323">
   <si>
     <t>Date:</t>
   </si>
@@ -1569,6 +1569,22 @@
   <si>
     <t>For some enemy types that used the charge enemy script but didn't have the charge enemy animation components, nullreference errors where thrown for each enemy present in the scene trying to access nonexistent animation components
 RESOLVED: added a check for charge enemy script (and future enmy types with animations) to to see if animation components are needed or not</t>
+  </si>
+  <si>
+    <t>Player Level Up/Save Correction</t>
+  </si>
+  <si>
+    <t>Designing the method for increasing stats on level up/
+correcting player saves not saving</t>
+  </si>
+  <si>
+    <t>UI/Sprite creation</t>
+  </si>
+  <si>
+    <t>Checking to make sure that implementation of player leveling up is correct</t>
+  </si>
+  <si>
+    <t>Reviewing Player Level Up</t>
   </si>
 </sst>
 </file>
@@ -2057,7 +2073,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2323,6 +2339,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2690,8 +2709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2744,7 +2763,9 @@
       <c r="E6" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="F6" s="73"/>
+      <c r="F6" s="73" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="7" spans="2:7" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B7" s="72" t="s">
@@ -3332,9 +3353,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21:G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3378,7 +3399,7 @@
       <c r="C3" s="57"/>
       <c r="H3" s="79">
         <f>SUM(G12:G118)</f>
-        <v>0.47222222222222249</v>
+        <v>1.8055555555555935E-2</v>
       </c>
       <c r="I3" t="s">
         <v>187</v>
@@ -3391,7 +3412,7 @@
       <c r="C4" s="27"/>
       <c r="H4" s="80">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>11.333333333333334</v>
+        <v>0.43333333333333335</v>
       </c>
       <c r="I4" t="s">
         <v>187</v>
@@ -3726,16 +3747,49 @@
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C22" s="3">
+        <v>42124</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.4458333333333333</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.5541666666666667</v>
+      </c>
       <c r="G22" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.10833333333333339</v>
+      </c>
+      <c r="H22" t="s">
+        <v>318</v>
+      </c>
+      <c r="I22" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="112" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="3">
+        <v>42124</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.5625</v>
+      </c>
       <c r="G23" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.5625</v>
+      </c>
+      <c r="H23" t="s">
+        <v>322</v>
+      </c>
+      <c r="I23" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
@@ -4333,7 +4387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
     </sheetView>
@@ -6199,42 +6253,42 @@
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
-      <c r="N6" s="112"/>
-      <c r="O6" s="112"/>
-      <c r="P6" s="112"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="113"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="113"/>
+      <c r="K6" s="113"/>
+      <c r="L6" s="113"/>
+      <c r="M6" s="113"/>
+      <c r="N6" s="113"/>
+      <c r="O6" s="113"/>
+      <c r="P6" s="113"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="112"/>
-      <c r="N7" s="112"/>
-      <c r="O7" s="112"/>
-      <c r="P7" s="112"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="113"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="113"/>
+      <c r="M7" s="113"/>
+      <c r="N7" s="113"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="113"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -6245,55 +6299,55 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="112"/>
-      <c r="I10" s="112"/>
-      <c r="J10" s="112"/>
-      <c r="K10" s="112"/>
-      <c r="L10" s="112"/>
-      <c r="M10" s="112"/>
-      <c r="N10" s="112"/>
-      <c r="O10" s="112"/>
-      <c r="P10" s="112"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="113"/>
+      <c r="K10" s="113"/>
+      <c r="L10" s="113"/>
+      <c r="M10" s="113"/>
+      <c r="N10" s="113"/>
+      <c r="O10" s="113"/>
+      <c r="P10" s="113"/>
     </row>
     <row r="11" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="112"/>
-      <c r="E11" s="112"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="112"/>
-      <c r="H11" s="112"/>
-      <c r="I11" s="112"/>
-      <c r="J11" s="112"/>
-      <c r="K11" s="112"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="113"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="113"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="112"/>
-      <c r="F12" s="112"/>
-      <c r="G12" s="112"/>
-      <c r="H12" s="112"/>
-      <c r="I12" s="112"/>
-      <c r="J12" s="112"/>
-      <c r="K12" s="112"/>
-      <c r="L12" s="112"/>
-      <c r="M12" s="112"/>
-      <c r="N12" s="112"/>
-      <c r="O12" s="112"/>
-      <c r="P12" s="112"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="113"/>
+      <c r="I12" s="113"/>
+      <c r="J12" s="113"/>
+      <c r="K12" s="113"/>
+      <c r="L12" s="113"/>
+      <c r="M12" s="113"/>
+      <c r="N12" s="113"/>
+      <c r="O12" s="113"/>
+      <c r="P12" s="113"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="11" t="s">
@@ -6301,36 +6355,36 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="112" t="s">
+      <c r="B14" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="112"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="112"/>
-      <c r="H14" s="112"/>
-      <c r="I14" s="112"/>
-      <c r="J14" s="112"/>
-      <c r="K14" s="112"/>
-      <c r="L14" s="112"/>
-      <c r="M14" s="112"/>
-      <c r="N14" s="112"/>
-      <c r="O14" s="112"/>
+      <c r="C14" s="113"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="113"/>
+      <c r="J14" s="113"/>
+      <c r="K14" s="113"/>
+      <c r="L14" s="113"/>
+      <c r="M14" s="113"/>
+      <c r="N14" s="113"/>
+      <c r="O14" s="113"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="114" t="s">
+      <c r="C15" s="115" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="112"/>
-      <c r="E15" s="112"/>
-      <c r="F15" s="112"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="112"/>
-      <c r="I15" s="112"/>
-      <c r="J15" s="112"/>
-      <c r="K15" s="112"/>
-      <c r="L15" s="112"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
+      <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16" s="12"/>
@@ -6361,187 +6415,187 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="116" t="s">
+      <c r="C18" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="112"/>
-      <c r="I18" s="112"/>
-      <c r="J18" s="112"/>
-      <c r="K18" s="112"/>
-      <c r="L18" s="112"/>
-      <c r="M18" s="112"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="113"/>
+      <c r="I18" s="113"/>
+      <c r="J18" s="113"/>
+      <c r="K18" s="113"/>
+      <c r="L18" s="113"/>
+      <c r="M18" s="113"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="115" t="s">
+      <c r="D19" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="112"/>
-      <c r="F19" s="112"/>
-      <c r="G19" s="112"/>
-      <c r="H19" s="112"/>
-      <c r="I19" s="112"/>
-      <c r="J19" s="112"/>
-      <c r="K19" s="112"/>
-      <c r="L19" s="112"/>
-      <c r="M19" s="112"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="113"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="113"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="113"/>
+      <c r="L19" s="113"/>
+      <c r="M19" s="113"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
-      <c r="C20" s="115" t="s">
+      <c r="C20" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="112"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="112"/>
-      <c r="I20" s="112"/>
-      <c r="J20" s="112"/>
-      <c r="K20" s="112"/>
-      <c r="L20" s="112"/>
-      <c r="M20" s="112"/>
+      <c r="D20" s="113"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="113"/>
+      <c r="G20" s="113"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="113"/>
+      <c r="K20" s="113"/>
+      <c r="L20" s="113"/>
+      <c r="M20" s="113"/>
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="112" t="s">
+      <c r="D21" s="113" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="112"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="112"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="112"/>
-      <c r="K21" s="112"/>
-      <c r="L21" s="112"/>
-      <c r="M21" s="112"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="113"/>
+      <c r="L21" s="113"/>
+      <c r="M21" s="113"/>
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="112" t="s">
+      <c r="D22" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="112"/>
-      <c r="F22" s="112"/>
-      <c r="G22" s="112"/>
-      <c r="H22" s="112"/>
-      <c r="I22" s="112"/>
-      <c r="J22" s="112"/>
-      <c r="K22" s="112"/>
-      <c r="L22" s="112"/>
-      <c r="M22" s="112"/>
-      <c r="N22" s="112"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="113"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="113"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="113"/>
+      <c r="K22" s="113"/>
+      <c r="L22" s="113"/>
+      <c r="M22" s="113"/>
+      <c r="N22" s="113"/>
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="112" t="s">
+      <c r="D23" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="112"/>
-      <c r="F23" s="112"/>
-      <c r="G23" s="112"/>
-      <c r="H23" s="112"/>
-      <c r="I23" s="112"/>
-      <c r="J23" s="112"/>
-      <c r="K23" s="112"/>
-      <c r="L23" s="112"/>
-      <c r="M23" s="112"/>
-      <c r="N23" s="112"/>
-      <c r="O23" s="112"/>
-      <c r="P23" s="112"/>
-      <c r="Q23" s="112"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="113"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="113"/>
+      <c r="M23" s="113"/>
+      <c r="N23" s="113"/>
+      <c r="O23" s="113"/>
+      <c r="P23" s="113"/>
+      <c r="Q23" s="113"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="112" t="s">
+      <c r="D24" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="112"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="112"/>
-      <c r="H24" s="112"/>
-      <c r="I24" s="112"/>
-      <c r="J24" s="112"/>
-      <c r="K24" s="112"/>
-      <c r="L24" s="112"/>
-      <c r="M24" s="112"/>
-      <c r="N24" s="112"/>
-      <c r="O24" s="112"/>
-      <c r="P24" s="112"/>
-      <c r="Q24" s="112"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="113"/>
+      <c r="G24" s="113"/>
+      <c r="H24" s="113"/>
+      <c r="I24" s="113"/>
+      <c r="J24" s="113"/>
+      <c r="K24" s="113"/>
+      <c r="L24" s="113"/>
+      <c r="M24" s="113"/>
+      <c r="N24" s="113"/>
+      <c r="O24" s="113"/>
+      <c r="P24" s="113"/>
+      <c r="Q24" s="113"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="112" t="s">
+      <c r="D25" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="112"/>
-      <c r="F25" s="112"/>
-      <c r="G25" s="112"/>
-      <c r="H25" s="112"/>
-      <c r="I25" s="112"/>
-      <c r="J25" s="112"/>
-      <c r="K25" s="112"/>
-      <c r="L25" s="112"/>
-      <c r="M25" s="112"/>
-      <c r="N25" s="112"/>
-      <c r="O25" s="112"/>
-      <c r="P25" s="112"/>
-      <c r="Q25" s="112"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="113"/>
+      <c r="G25" s="113"/>
+      <c r="H25" s="113"/>
+      <c r="I25" s="113"/>
+      <c r="J25" s="113"/>
+      <c r="K25" s="113"/>
+      <c r="L25" s="113"/>
+      <c r="M25" s="113"/>
+      <c r="N25" s="113"/>
+      <c r="O25" s="113"/>
+      <c r="P25" s="113"/>
+      <c r="Q25" s="113"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
-      <c r="C26" s="115" t="s">
+      <c r="C26" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="112"/>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="112"/>
-      <c r="H26" s="112"/>
-      <c r="I26" s="112"/>
-      <c r="J26" s="112"/>
-      <c r="K26" s="112"/>
-      <c r="L26" s="112"/>
-      <c r="M26" s="112"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="113"/>
+      <c r="F26" s="113"/>
+      <c r="G26" s="113"/>
+      <c r="H26" s="113"/>
+      <c r="I26" s="113"/>
+      <c r="J26" s="113"/>
+      <c r="K26" s="113"/>
+      <c r="L26" s="113"/>
+      <c r="M26" s="113"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="112" t="s">
+      <c r="D27" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="112"/>
-      <c r="F27" s="112"/>
-      <c r="G27" s="112"/>
-      <c r="H27" s="112"/>
-      <c r="I27" s="112"/>
-      <c r="J27" s="112"/>
-      <c r="K27" s="112"/>
-      <c r="L27" s="112"/>
-      <c r="M27" s="112"/>
+      <c r="E27" s="113"/>
+      <c r="F27" s="113"/>
+      <c r="G27" s="113"/>
+      <c r="H27" s="113"/>
+      <c r="I27" s="113"/>
+      <c r="J27" s="113"/>
+      <c r="K27" s="113"/>
+      <c r="L27" s="113"/>
+      <c r="M27" s="113"/>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
     </row>
@@ -6572,84 +6626,84 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="114" t="s">
+      <c r="C32" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="112"/>
-      <c r="E32" s="112"/>
-      <c r="F32" s="112"/>
-      <c r="G32" s="112"/>
-      <c r="H32" s="112"/>
-      <c r="I32" s="112"/>
-      <c r="J32" s="112"/>
-      <c r="K32" s="112"/>
-      <c r="L32" s="112"/>
-      <c r="M32" s="112"/>
-      <c r="N32" s="112"/>
+      <c r="D32" s="113"/>
+      <c r="E32" s="113"/>
+      <c r="F32" s="113"/>
+      <c r="G32" s="113"/>
+      <c r="H32" s="113"/>
+      <c r="I32" s="113"/>
+      <c r="J32" s="113"/>
+      <c r="K32" s="113"/>
+      <c r="L32" s="113"/>
+      <c r="M32" s="113"/>
+      <c r="N32" s="113"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C34" s="112" t="s">
+      <c r="C34" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="112"/>
-      <c r="H34" s="112"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="112"/>
-      <c r="K34" s="112"/>
-      <c r="L34" s="112"/>
-      <c r="M34" s="112"/>
-      <c r="N34" s="112"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="113"/>
+      <c r="H34" s="113"/>
+      <c r="I34" s="113"/>
+      <c r="J34" s="113"/>
+      <c r="K34" s="113"/>
+      <c r="L34" s="113"/>
+      <c r="M34" s="113"/>
+      <c r="N34" s="113"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C35" s="114" t="s">
+      <c r="C35" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="112"/>
-      <c r="E35" s="112"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="112"/>
-      <c r="H35" s="112"/>
-      <c r="I35" s="112"/>
-      <c r="J35" s="112"/>
-      <c r="K35" s="112"/>
-      <c r="L35" s="112"/>
-      <c r="M35" s="112"/>
-      <c r="N35" s="112"/>
+      <c r="D35" s="113"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="113"/>
+      <c r="G35" s="113"/>
+      <c r="H35" s="113"/>
+      <c r="I35" s="113"/>
+      <c r="J35" s="113"/>
+      <c r="K35" s="113"/>
+      <c r="L35" s="113"/>
+      <c r="M35" s="113"/>
+      <c r="N35" s="113"/>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C37" s="112" t="s">
+      <c r="C37" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="112"/>
-      <c r="E37" s="112"/>
-      <c r="F37" s="112"/>
-      <c r="G37" s="112"/>
-      <c r="H37" s="112"/>
-      <c r="I37" s="112"/>
-      <c r="J37" s="112"/>
-      <c r="K37" s="112"/>
-      <c r="L37" s="112"/>
-      <c r="M37" s="112"/>
-      <c r="N37" s="112"/>
+      <c r="D37" s="113"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="113"/>
+      <c r="G37" s="113"/>
+      <c r="H37" s="113"/>
+      <c r="I37" s="113"/>
+      <c r="J37" s="113"/>
+      <c r="K37" s="113"/>
+      <c r="L37" s="113"/>
+      <c r="M37" s="113"/>
+      <c r="N37" s="113"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C38" s="114" t="s">
+      <c r="C38" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="112"/>
-      <c r="E38" s="112"/>
-      <c r="F38" s="112"/>
-      <c r="G38" s="112"/>
-      <c r="H38" s="112"/>
-      <c r="I38" s="112"/>
-      <c r="J38" s="112"/>
-      <c r="K38" s="112"/>
-      <c r="L38" s="112"/>
-      <c r="M38" s="112"/>
-      <c r="N38" s="112"/>
+      <c r="D38" s="113"/>
+      <c r="E38" s="113"/>
+      <c r="F38" s="113"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="113"/>
+      <c r="I38" s="113"/>
+      <c r="J38" s="113"/>
+      <c r="K38" s="113"/>
+      <c r="L38" s="113"/>
+      <c r="M38" s="113"/>
+      <c r="N38" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="22">

</xml_diff>

<commit_message>
Added Quit button image; unversioned char1 save
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
@@ -3355,7 +3355,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3399,7 +3399,7 @@
       <c r="C3" s="57"/>
       <c r="H3" s="79">
         <f>SUM(G12:G118)</f>
-        <v>1.8055555555555935E-2</v>
+        <v>0.59583333333333377</v>
       </c>
       <c r="I3" t="s">
         <v>187</v>
@@ -3412,7 +3412,7 @@
       <c r="C4" s="27"/>
       <c r="H4" s="80">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>0.43333333333333335</v>
+        <v>14.3</v>
       </c>
       <c r="I4" t="s">
         <v>187</v>
@@ -3778,9 +3778,12 @@
       <c r="D23" s="5">
         <v>0.5625</v>
       </c>
+      <c r="E23" s="5">
+        <v>0.57777777777777783</v>
+      </c>
       <c r="G23" s="8">
         <f t="shared" si="0"/>
-        <v>-0.5625</v>
+        <v>1.5277777777777835E-2</v>
       </c>
       <c r="H23" t="s">
         <v>322</v>

</xml_diff>

<commit_message>
Updated berserk/charge enemy types to used idle sprite as base image; Text on EXP bar is black now; lowered volume in game scene to 0.5; starting stats/growth rates for each class altered
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_rsanders_timelog.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="325">
   <si>
     <t>Date:</t>
   </si>
@@ -1585,6 +1585,12 @@
   </si>
   <si>
     <t>Reviewing Player Level Up</t>
+  </si>
+  <si>
+    <t>Player Class Balancing</t>
+  </si>
+  <si>
+    <t>Playing through the game and reassessing appropriate growth rates based on ease of using a certain class</t>
   </si>
 </sst>
 </file>
@@ -2350,12 +2356,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
@@ -3355,7 +3361,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3399,7 +3405,7 @@
       <c r="C3" s="57"/>
       <c r="H3" s="79">
         <f>SUM(G12:G118)</f>
-        <v>0.59583333333333377</v>
+        <v>0.64513888888888937</v>
       </c>
       <c r="I3" t="s">
         <v>187</v>
@@ -3412,7 +3418,7 @@
       <c r="C4" s="27"/>
       <c r="H4" s="80">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>14.3</v>
+        <v>15.483333333333333</v>
       </c>
       <c r="I4" t="s">
         <v>187</v>
@@ -3796,9 +3802,27 @@
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="3">
+        <v>42124</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.65347222222222223</v>
+      </c>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.9305555555555602E-2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>323</v>
+      </c>
+      <c r="I24" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
@@ -6321,7 +6345,7 @@
       <c r="P10" s="113"/>
     </row>
     <row r="11" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="114" t="s">
+      <c r="C11" s="117" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="113"/>
@@ -6376,7 +6400,7 @@
       <c r="O14" s="113"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="115" t="s">
+      <c r="C15" s="114" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="113"/>
@@ -6418,7 +6442,7 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="117" t="s">
+      <c r="C18" s="116" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="113"/>
@@ -6437,7 +6461,7 @@
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="116" t="s">
+      <c r="D19" s="115" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="113"/>
@@ -6454,7 +6478,7 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
-      <c r="C20" s="116" t="s">
+      <c r="C20" s="115" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="113"/>
@@ -6568,7 +6592,7 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
-      <c r="C26" s="116" t="s">
+      <c r="C26" s="115" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="113"/>
@@ -6629,7 +6653,7 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="115" t="s">
+      <c r="C32" s="114" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="113"/>
@@ -6661,7 +6685,7 @@
       <c r="N34" s="113"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C35" s="115" t="s">
+      <c r="C35" s="114" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="113"/>
@@ -6693,7 +6717,7 @@
       <c r="N37" s="113"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C38" s="115" t="s">
+      <c r="C38" s="114" t="s">
         <v>25</v>
       </c>
       <c r="D38" s="113"/>
@@ -6710,6 +6734,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="D25:Q25"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="B10:P10"/>
+    <mergeCell ref="B12:P12"/>
     <mergeCell ref="C34:N34"/>
     <mergeCell ref="C35:N35"/>
     <mergeCell ref="C37:N37"/>
@@ -6726,12 +6756,6 @@
     <mergeCell ref="D22:N22"/>
     <mergeCell ref="D23:Q23"/>
     <mergeCell ref="D24:Q24"/>
-    <mergeCell ref="D25:Q25"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="B7:P7"/>
-    <mergeCell ref="B10:P10"/>
-    <mergeCell ref="B12:P12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1"/>

</xml_diff>